<commit_message>
Minor tweaks to DH tabs
</commit_message>
<xml_diff>
--- a/doc/notes/Cryptography.xlsx
+++ b/doc/notes/Cryptography.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\doc\crypto\doc\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACC630E-F6AC-4222-9222-C4D51A9389E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855F156E-82E0-4C3E-9F3E-433F92195D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15540" firstSheet="2" activeTab="10" xr2:uid="{6349FD4F-D13B-4095-B9BB-C39254E42942}"/>
   </bookViews>
@@ -4954,7 +4954,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4998,11 +4998,11 @@
         <v>7</v>
       </c>
       <c r="D2" s="64">
-        <f>C2*B2+1</f>
+        <f t="shared" ref="D2:D29" si="0">C2*B2+1</f>
         <v>29</v>
       </c>
       <c r="E2" s="64">
-        <f>MOD(POWER(A2,B2),D2)</f>
+        <f t="shared" ref="E2:E29" si="1">MOD(POWER(A2,B2),D2)</f>
         <v>1</v>
       </c>
       <c r="F2" s="64">
@@ -5010,7 +5010,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="64">
-        <f>MOD(POWER(F2,C2),D2)</f>
+        <f t="shared" ref="G2:G29" si="2">MOD(POWER(F2,C2),D2)</f>
         <v>1</v>
       </c>
     </row>
@@ -5021,23 +5021,23 @@
       <c r="B3" s="65">
         <v>4</v>
       </c>
-      <c r="C3" s="65">
+      <c r="C3" s="64">
         <v>7</v>
       </c>
       <c r="D3" s="65">
-        <f>C3*B3+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E3" s="65">
-        <f>MOD(POWER(A3,B3),D3)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="F3" s="65">
-        <f t="shared" ref="F3:F30" si="0">E3</f>
+        <f t="shared" ref="F3:F29" si="3">E3</f>
         <v>16</v>
       </c>
       <c r="G3" s="65">
-        <f>MOD(POWER(F3,C3),D3)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5048,23 +5048,23 @@
       <c r="B4" s="65">
         <v>4</v>
       </c>
-      <c r="C4" s="65">
+      <c r="C4" s="64">
         <v>7</v>
       </c>
       <c r="D4" s="65">
-        <f>C4*B4+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E4" s="65">
-        <f>MOD(POWER(A4,B4),D4)</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="F4" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="G4" s="65">
-        <f>MOD(POWER(F4,C4),D4)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5075,23 +5075,23 @@
       <c r="B5" s="65">
         <v>4</v>
       </c>
-      <c r="C5" s="65">
+      <c r="C5" s="64">
         <v>7</v>
       </c>
       <c r="D5" s="65">
-        <f>C5*B5+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E5" s="65">
-        <f>MOD(POWER(A5,B5),D5)</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="F5" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="G5" s="65">
-        <f>MOD(POWER(F5,C5),D5)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5102,23 +5102,23 @@
       <c r="B6" s="65">
         <v>4</v>
       </c>
-      <c r="C6" s="65">
+      <c r="C6" s="64">
         <v>7</v>
       </c>
       <c r="D6" s="65">
-        <f>C6*B6+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E6" s="65">
-        <f>MOD(POWER(A6,B6),D6)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="F6" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="G6" s="65">
-        <f>MOD(POWER(F6,C6),D6)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5129,23 +5129,23 @@
       <c r="B7" s="65">
         <v>4</v>
       </c>
-      <c r="C7" s="65">
+      <c r="C7" s="64">
         <v>7</v>
       </c>
       <c r="D7" s="65">
-        <f>C7*B7+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E7" s="65">
-        <f>MOD(POWER(A7,B7),D7)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="F7" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="G7" s="65">
-        <f>MOD(POWER(F7,C7),D7)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5156,23 +5156,23 @@
       <c r="B8" s="65">
         <v>4</v>
       </c>
-      <c r="C8" s="65">
+      <c r="C8" s="64">
         <v>7</v>
       </c>
       <c r="D8" s="65">
-        <f>C8*B8+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E8" s="65">
-        <f>MOD(POWER(A8,B8),D8)</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="F8" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="G8" s="65">
-        <f>MOD(POWER(F8,C8),D8)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5183,23 +5183,23 @@
       <c r="B9" s="65">
         <v>4</v>
       </c>
-      <c r="C9" s="65">
+      <c r="C9" s="64">
         <v>7</v>
       </c>
       <c r="D9" s="65">
-        <f>C9*B9+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E9" s="65">
-        <f>MOD(POWER(A9,B9),D9)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="F9" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="G9" s="65">
-        <f>MOD(POWER(F9,C9),D9)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5210,23 +5210,23 @@
       <c r="B10" s="65">
         <v>4</v>
       </c>
-      <c r="C10" s="65">
+      <c r="C10" s="64">
         <v>7</v>
       </c>
       <c r="D10" s="65">
-        <f>C10*B10+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E10" s="65">
-        <f>MOD(POWER(A10,B10),D10)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="F10" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="G10" s="65">
-        <f>MOD(POWER(F10,C10),D10)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5237,23 +5237,23 @@
       <c r="B11" s="65">
         <v>4</v>
       </c>
-      <c r="C11" s="65">
+      <c r="C11" s="64">
         <v>7</v>
       </c>
       <c r="D11" s="65">
-        <f>C11*B11+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E11" s="65">
-        <f>MOD(POWER(A11,B11),D11)</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="F11" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="G11" s="65">
-        <f>MOD(POWER(F11,C11),D11)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5264,23 +5264,23 @@
       <c r="B12" s="65">
         <v>4</v>
       </c>
-      <c r="C12" s="65">
+      <c r="C12" s="64">
         <v>7</v>
       </c>
       <c r="D12" s="65">
-        <f>C12*B12+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E12" s="65">
-        <f>MOD(POWER(A12,B12),D12)</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="F12" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="G12" s="65">
-        <f>MOD(POWER(F12,C12),D12)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5295,19 +5295,19 @@
         <v>7</v>
       </c>
       <c r="D13" s="64">
-        <f>C13*B13+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E13" s="64">
-        <f>MOD(POWER(A13,B13),D13)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="F13" s="64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G13" s="64">
-        <f>MOD(POWER(F13,C13),D13)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5318,23 +5318,23 @@
       <c r="B14" s="65">
         <v>4</v>
       </c>
-      <c r="C14" s="65">
+      <c r="C14" s="64">
         <v>7</v>
       </c>
       <c r="D14" s="65">
-        <f>C14*B14+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E14" s="65">
-        <f>MOD(POWER(A14,B14),D14)</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="F14" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="G14" s="65">
-        <f>MOD(POWER(F14,C14),D14)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5345,23 +5345,23 @@
       <c r="B15" s="65">
         <v>4</v>
       </c>
-      <c r="C15" s="65">
+      <c r="C15" s="64">
         <v>7</v>
       </c>
       <c r="D15" s="65">
-        <f>C15*B15+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E15" s="65">
-        <f>MOD(POWER(A15,B15),D15)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="F15" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="G15" s="65">
-        <f>MOD(POWER(F15,C15),D15)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5372,23 +5372,23 @@
       <c r="B16" s="65">
         <v>4</v>
       </c>
-      <c r="C16" s="65">
+      <c r="C16" s="64">
         <v>7</v>
       </c>
       <c r="D16" s="65">
-        <f>C16*B16+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E16" s="65">
-        <f>MOD(POWER(A16,B16),D16)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="F16" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="G16" s="65">
-        <f>MOD(POWER(F16,C16),D16)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5399,23 +5399,23 @@
       <c r="B17" s="65">
         <v>4</v>
       </c>
-      <c r="C17" s="65">
+      <c r="C17" s="64">
         <v>7</v>
       </c>
       <c r="D17" s="65">
-        <f>C17*B17+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E17" s="65">
-        <f>MOD(POWER(A17,B17),D17)</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="F17" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="G17" s="65">
-        <f>MOD(POWER(F17,C17),D17)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5430,19 +5430,19 @@
         <v>7</v>
       </c>
       <c r="D18" s="64">
-        <f>C18*B18+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E18" s="64">
-        <f>MOD(POWER(A18,B18),D18)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="F18" s="64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G18" s="64">
-        <f>MOD(POWER(F18,C18),D18)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5453,23 +5453,23 @@
       <c r="B19" s="65">
         <v>4</v>
       </c>
-      <c r="C19" s="65">
+      <c r="C19" s="64">
         <v>7</v>
       </c>
       <c r="D19" s="65">
-        <f>C19*B19+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E19" s="65">
-        <f>MOD(POWER(A19,B19),D19)</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="F19" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="G19" s="65">
-        <f>MOD(POWER(F19,C19),D19)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5480,23 +5480,23 @@
       <c r="B20" s="65">
         <v>4</v>
       </c>
-      <c r="C20" s="65">
+      <c r="C20" s="64">
         <v>7</v>
       </c>
       <c r="D20" s="65">
-        <f>C20*B20+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E20" s="65">
-        <f>MOD(POWER(A20,B20),D20)</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="F20" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="G20" s="65">
-        <f>MOD(POWER(F20,C20),D20)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5507,23 +5507,23 @@
       <c r="B21" s="65">
         <v>4</v>
       </c>
-      <c r="C21" s="65">
+      <c r="C21" s="64">
         <v>7</v>
       </c>
       <c r="D21" s="65">
-        <f>C21*B21+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E21" s="65">
-        <f>MOD(POWER(A21,B21),D21)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="F21" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="G21" s="65">
-        <f>MOD(POWER(F21,C21),D21)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5534,23 +5534,23 @@
       <c r="B22" s="65">
         <v>4</v>
       </c>
-      <c r="C22" s="65">
+      <c r="C22" s="64">
         <v>7</v>
       </c>
       <c r="D22" s="65">
-        <f>C22*B22+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E22" s="65">
-        <f>MOD(POWER(A22,B22),D22)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="F22" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="G22" s="65">
-        <f>MOD(POWER(F22,C22),D22)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5561,23 +5561,23 @@
       <c r="B23" s="65">
         <v>4</v>
       </c>
-      <c r="C23" s="65">
+      <c r="C23" s="64">
         <v>7</v>
       </c>
       <c r="D23" s="65">
-        <f>C23*B23+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E23" s="65">
-        <f>MOD(POWER(A23,B23),D23)</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="F23" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="G23" s="65">
-        <f>MOD(POWER(F23,C23),D23)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5588,23 +5588,23 @@
       <c r="B24" s="65">
         <v>4</v>
       </c>
-      <c r="C24" s="65">
+      <c r="C24" s="64">
         <v>7</v>
       </c>
       <c r="D24" s="65">
-        <f>C24*B24+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E24" s="65">
-        <f>MOD(POWER(A24,B24),D24)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="F24" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="G24" s="65">
-        <f>MOD(POWER(F24,C24),D24)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5615,23 +5615,23 @@
       <c r="B25" s="65">
         <v>4</v>
       </c>
-      <c r="C25" s="65">
+      <c r="C25" s="64">
         <v>7</v>
       </c>
       <c r="D25" s="65">
-        <f>C25*B25+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E25" s="65">
-        <f>MOD(POWER(A25,B25),D25)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="F25" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="G25" s="65">
-        <f>MOD(POWER(F25,C25),D25)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5642,23 +5642,23 @@
       <c r="B26" s="65">
         <v>4</v>
       </c>
-      <c r="C26" s="65">
+      <c r="C26" s="64">
         <v>7</v>
       </c>
       <c r="D26" s="65">
-        <f>C26*B26+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E26" s="65">
-        <f>MOD(POWER(A26,B26),D26)</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="F26" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="G26" s="65">
-        <f>MOD(POWER(F26,C26),D26)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5669,23 +5669,23 @@
       <c r="B27" s="65">
         <v>4</v>
       </c>
-      <c r="C27" s="65">
+      <c r="C27" s="64">
         <v>7</v>
       </c>
       <c r="D27" s="65">
-        <f>C27*B27+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E27" s="65">
-        <f>MOD(POWER(A27,B27),D27)</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="F27" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="G27" s="65">
-        <f>MOD(POWER(F27,C27),D27)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5696,23 +5696,23 @@
       <c r="B28" s="65">
         <v>4</v>
       </c>
-      <c r="C28" s="65">
+      <c r="C28" s="64">
         <v>7</v>
       </c>
       <c r="D28" s="65">
-        <f>C28*B28+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E28" s="65">
-        <f>MOD(POWER(A28,B28),D28)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="F28" s="65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="G28" s="65">
-        <f>MOD(POWER(F28,C28),D28)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5727,19 +5727,19 @@
         <v>7</v>
       </c>
       <c r="D29" s="64">
-        <f>C29*B29+1</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="E29" s="64">
-        <f>MOD(POWER(A29,B29),D29)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="F29" s="64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G29" s="64">
-        <f>MOD(POWER(F29,C29),D29)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5758,7 +5758,7 @@
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="D35" sqref="D35"/>
-      <selection pane="topRight" activeCell="R9" sqref="R9"/>
+      <selection pane="topRight" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6122,7 +6122,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B5:K31" si="2">MOD(POWER($A5,B$2),29)</f>
+        <f t="shared" ref="B5:L31" si="2">MOD(POWER($A5,B$2),29)</f>
         <v>3</v>
       </c>
       <c r="C5">
@@ -6652,55 +6652,55 @@
         <v>7</v>
       </c>
       <c r="Q9" s="65">
-        <f>MOD(POWER($A9,MOD(Q$2,$H$2)),29)</f>
+        <f t="shared" ref="Q9:AC9" si="3">MOD(POWER($A9,MOD(Q$2,$H$2)),29)</f>
         <v>20</v>
       </c>
       <c r="R9" s="65">
-        <f>MOD(POWER($A9,MOD(R$2,$H$2)),29)</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="S9" s="65">
-        <f>MOD(POWER($A9,MOD(S$2,$H$2)),29)</f>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="T9" s="65">
-        <f>MOD(POWER($A9,MOD(T$2,$H$2)),29)</f>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="U9" s="65">
-        <f>MOD(POWER($A9,MOD(U$2,$H$2)),29)</f>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="V9" s="65">
-        <f>MOD(POWER($A9,MOD(V$2,$H$2)),29)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="W9" s="65">
-        <f>MOD(POWER($A9,MOD(W$2,$H$2)),29)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="X9" s="65">
-        <f>MOD(POWER($A9,MOD(X$2,$H$2)),29)</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="Y9" s="65">
-        <f>MOD(POWER($A9,MOD(Y$2,$H$2)),29)</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="Z9" s="65">
-        <f>MOD(POWER($A9,MOD(Z$2,$H$2)),29)</f>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="AA9" s="65">
-        <f>MOD(POWER($A9,MOD(AA$2,$H$2)),29)</f>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="AB9" s="65">
-        <f>MOD(POWER($A9,MOD(AB$2,$H$2)),29)</f>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="AC9" s="65">
-        <f>MOD(POWER($A9,MOD(AC$2,$H$2)),29)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="AD9" s="65">
@@ -7627,57 +7627,75 @@
         <v>25</v>
       </c>
       <c r="M18" s="65">
+        <f>MOD(POWER($A18,MOD(M$2,$H$2)),29)</f>
         <v>23</v>
       </c>
       <c r="N18" s="65">
+        <f>MOD(POWER($A18,MOD(N$2,$H$2)),29)</f>
         <v>20</v>
       </c>
       <c r="O18" s="65">
+        <f>MOD(POWER($A18,MOD(O$2,$H$2)),29)</f>
         <v>1</v>
       </c>
       <c r="P18" s="65">
+        <f>MOD(POWER($A18,MOD(P$2,$H$2)),29)</f>
         <v>16</v>
       </c>
       <c r="Q18" s="65">
+        <f>MOD(POWER($A18,MOD(Q$2,$H$2)),29)</f>
         <v>24</v>
       </c>
       <c r="R18" s="65">
+        <f>MOD(POWER($A18,MOD(R$2,$H$2)),29)</f>
         <v>7</v>
       </c>
       <c r="S18" s="65">
+        <f>MOD(POWER($A18,MOD(S$2,$H$2)),29)</f>
         <v>25</v>
       </c>
       <c r="T18" s="65">
+        <f>MOD(POWER($A18,MOD(T$2,$H$2)),29)</f>
         <v>23</v>
       </c>
       <c r="U18" s="65">
+        <f>MOD(POWER($A18,MOD(U$2,$H$2)),29)</f>
         <v>20</v>
       </c>
       <c r="V18" s="65">
+        <f>MOD(POWER($A18,MOD(V$2,$H$2)),29)</f>
         <v>1</v>
       </c>
       <c r="W18" s="65">
+        <f>MOD(POWER($A18,MOD(W$2,$H$2)),29)</f>
         <v>16</v>
       </c>
       <c r="X18" s="65">
+        <f>MOD(POWER($A18,MOD(X$2,$H$2)),29)</f>
         <v>24</v>
       </c>
       <c r="Y18" s="65">
+        <f>MOD(POWER($A18,MOD(Y$2,$H$2)),29)</f>
         <v>7</v>
       </c>
       <c r="Z18" s="65">
+        <f>MOD(POWER($A18,MOD(Z$2,$H$2)),29)</f>
         <v>25</v>
       </c>
       <c r="AA18" s="65">
+        <f>MOD(POWER($A18,MOD(AA$2,$H$2)),29)</f>
         <v>23</v>
       </c>
       <c r="AB18" s="65">
+        <f>MOD(POWER($A18,MOD(AB$2,$H$2)),29)</f>
         <v>20</v>
       </c>
       <c r="AC18" s="65">
+        <f>MOD(POWER($A18,MOD(AC$2,$H$2)),29)</f>
         <v>1</v>
       </c>
       <c r="AD18" s="65">
+        <f>MOD(POWER($A18,MOD(AD$2,$H$2)),29)</f>
         <v>16</v>
       </c>
       <c r="AE18">

</xml_diff>